<commit_message>
screen dump update to 20211126
</commit_message>
<xml_diff>
--- a/docs/traderecords/f6_20211129.xlsx
+++ b/docs/traderecords/f6_20211129.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="341">
   <si>
     <t>证券代码</t>
   </si>
@@ -241,15 +241,6 @@
     <t>002177</t>
   </si>
   <si>
-    <t>000725</t>
-  </si>
-  <si>
-    <t>000625</t>
-  </si>
-  <si>
-    <t>515330</t>
-  </si>
-  <si>
     <t>证券名称</t>
   </si>
   <si>
@@ -475,15 +466,6 @@
     <t>御银股份</t>
   </si>
   <si>
-    <t>京东方Ａ</t>
-  </si>
-  <si>
-    <t>长安汽车</t>
-  </si>
-  <si>
-    <t>天弘300</t>
-  </si>
-  <si>
     <t>方向</t>
   </si>
   <si>
@@ -799,18 +781,6 @@
     <t>6.33</t>
   </si>
   <si>
-    <t>14.35</t>
-  </si>
-  <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>0.80</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
     <t>成交时间</t>
   </si>
   <si>
@@ -1067,90 +1037,25 @@
   </si>
   <si>
     <t>2021-11-29 09:30:00.200</t>
-  </si>
-  <si>
-    <t>2021-11-29 08:47:47.100</t>
-  </si>
-  <si>
-    <t>2021-11-29 08:32:24.490</t>
-  </si>
-  <si>
-    <t>2021-11-29 08:22:20.600</t>
-  </si>
-  <si>
-    <t>2021-11-29 08:22:07.160</t>
-  </si>
-  <si>
-    <t>2021-11-29 08:18:26.540</t>
-  </si>
-  <si>
-    <t>2021-11-29 01:35:26.270</t>
-  </si>
-  <si>
-    <t>2021-11-29 01:35:26.180</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:50:37.410</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:45:34.930</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:38:09.510</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:36:47.820</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:33:29.370</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:32:28.700</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:22:26.010</t>
-  </si>
-  <si>
-    <t>2021-11-28 19:20:42.380</t>
-  </si>
-  <si>
-    <t>2021-11-28 18:11:13.250</t>
-  </si>
-  <si>
-    <t>2021-11-28 18:11:05.230</t>
-  </si>
-  <si>
-    <t>2021-11-28 11:35:17.100</t>
-  </si>
-  <si>
-    <t>2021-11-28 11:35:16.530</t>
-  </si>
-  <si>
-    <t>2021-11-28 01:35:25.530</t>
-  </si>
-  <si>
-    <t>2021-11-28 01:35:25.520</t>
-  </si>
-  <si>
-    <t>2021-11-27 17:02:43.120</t>
-  </si>
-  <si>
-    <t>2021-11-27 11:35:16.970</t>
-  </si>
-  <si>
-    <t>2021-11-27 11:35:16.900</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1178,7 +1083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1186,7 +1091,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1470,33 +1375,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:XFD120"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1504,22 +1411,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G2" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1527,22 +1434,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1550,22 +1457,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1573,22 +1480,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1596,22 +1503,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1619,22 +1526,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1642,22 +1549,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" t="s">
         <v>158</v>
       </c>
-      <c r="D8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" t="s">
-        <v>164</v>
-      </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G8" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1665,22 +1572,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G9" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1688,22 +1595,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" t="s">
         <v>160</v>
       </c>
-      <c r="E10" t="s">
-        <v>166</v>
-      </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G10" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1711,22 +1618,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" t="s">
         <v>160</v>
       </c>
-      <c r="E11" t="s">
-        <v>166</v>
-      </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G11" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1734,22 +1641,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G12" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1757,22 +1664,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G13" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1780,22 +1687,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G14" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1803,22 +1710,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" t="s">
         <v>160</v>
       </c>
-      <c r="E15" t="s">
-        <v>166</v>
-      </c>
       <c r="F15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G15" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1826,22 +1733,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G16" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1849,22 +1756,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F17" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G17" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1872,22 +1779,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F18" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G18" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1895,22 +1802,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G19" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1918,22 +1825,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G20" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1941,22 +1848,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F21" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G21" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1964,22 +1871,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F22" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G22" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1987,22 +1894,22 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" t="s">
         <v>158</v>
       </c>
-      <c r="D23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E23" t="s">
-        <v>164</v>
-      </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G23" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2010,22 +1917,22 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F24" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G24" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2033,22 +1940,22 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E25" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F25" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G25" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2056,22 +1963,22 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" t="s">
         <v>160</v>
       </c>
-      <c r="E26" t="s">
-        <v>166</v>
-      </c>
       <c r="F26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G26" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2079,22 +1986,22 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" t="s">
         <v>160</v>
       </c>
-      <c r="E27" t="s">
-        <v>166</v>
-      </c>
       <c r="F27" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G27" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2102,22 +2009,22 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G28" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2125,22 +2032,22 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F29" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G29" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2148,22 +2055,22 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D30" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" t="s">
         <v>160</v>
       </c>
-      <c r="E30" t="s">
-        <v>166</v>
-      </c>
       <c r="F30" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G30" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2171,22 +2078,22 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G31" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2194,22 +2101,22 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G32" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2217,22 +2124,22 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F33" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G33" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2240,22 +2147,22 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G34" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2263,22 +2170,22 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E35" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F35" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G35" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2286,22 +2193,22 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E36" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F36" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G36" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2309,22 +2216,22 @@
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F37" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G37" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2332,22 +2239,22 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F38" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G38" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2355,22 +2262,22 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G39" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2378,22 +2285,22 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F40" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G40" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2401,22 +2308,22 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G41" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2424,22 +2331,22 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F42" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G42" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2447,22 +2354,22 @@
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" t="s">
         <v>160</v>
       </c>
-      <c r="E43" t="s">
-        <v>166</v>
-      </c>
       <c r="F43" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="G43" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2470,22 +2377,22 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E44" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F44" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G44" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2493,22 +2400,22 @@
         <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E45" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F45" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G45" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2516,22 +2423,22 @@
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E46" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F46" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G46" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2539,22 +2446,22 @@
         <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E47" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F47" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G47" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2562,22 +2469,22 @@
         <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E48" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F48" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G48" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2585,22 +2492,22 @@
         <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F49" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G49" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2608,22 +2515,22 @@
         <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E50" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G50" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2631,22 +2538,22 @@
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E51" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F51" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G51" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2654,22 +2561,22 @@
         <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G52" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2677,22 +2584,22 @@
         <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E53" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F53" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G53" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2700,22 +2607,22 @@
         <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E54" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F54" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G54" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2723,22 +2630,22 @@
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E55" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F55" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G55" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2746,22 +2653,22 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" t="s">
         <v>158</v>
       </c>
-      <c r="D56" t="s">
-        <v>160</v>
-      </c>
-      <c r="E56" t="s">
-        <v>164</v>
-      </c>
       <c r="F56" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G56" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2769,22 +2676,22 @@
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E57" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F57" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G57" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2792,22 +2699,22 @@
         <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E58" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F58" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G58" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2815,22 +2722,22 @@
         <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" t="s">
         <v>160</v>
       </c>
-      <c r="E59" t="s">
-        <v>166</v>
-      </c>
       <c r="F59" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G59" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2838,22 +2745,22 @@
         <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" t="s">
         <v>158</v>
       </c>
-      <c r="D60" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60" t="s">
-        <v>164</v>
-      </c>
       <c r="F60" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G60" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2861,22 +2768,22 @@
         <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" t="s">
         <v>158</v>
       </c>
-      <c r="D61" t="s">
-        <v>160</v>
-      </c>
-      <c r="E61" t="s">
-        <v>164</v>
-      </c>
       <c r="F61" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G61" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2884,22 +2791,22 @@
         <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E62" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F62" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G62" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2907,22 +2814,22 @@
         <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F63" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G63" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2930,22 +2837,22 @@
         <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" t="s">
         <v>160</v>
       </c>
-      <c r="E64" t="s">
-        <v>166</v>
-      </c>
       <c r="F64" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G64" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2953,22 +2860,22 @@
         <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C65" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D65" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E65" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F65" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G65" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2976,22 +2883,22 @@
         <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E66" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F66" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G66" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2999,22 +2906,22 @@
         <v>53</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E67" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F67" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G67" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3022,22 +2929,22 @@
         <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E68" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F68" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G68" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3045,22 +2952,22 @@
         <v>54</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D69" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E69" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F69" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="G69" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3068,22 +2975,22 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E70" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F70" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G70" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3091,22 +2998,22 @@
         <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D71" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E71" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F71" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G71" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3114,22 +3021,22 @@
         <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E72" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F72" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G72" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3137,22 +3044,22 @@
         <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D73" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E73" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F73" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G73" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3160,22 +3067,22 @@
         <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E74" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F74" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G74" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3183,22 +3090,22 @@
         <v>59</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C75" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E75" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F75" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G75" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3206,22 +3113,22 @@
         <v>60</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C76" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E76" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F76" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G76" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3229,22 +3136,22 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D77" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F77" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="G77" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3252,22 +3159,22 @@
         <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E78" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F78" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G78" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3275,22 +3182,22 @@
         <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D79" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E79" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F79" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G79" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3298,22 +3205,22 @@
         <v>62</v>
       </c>
       <c r="B80" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D80" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E80" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F80" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G80" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3321,22 +3228,22 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D81" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E81" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F81" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G81" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3344,22 +3251,22 @@
         <v>63</v>
       </c>
       <c r="B82" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C82" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D82" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E82" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F82" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G82" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3367,22 +3274,22 @@
         <v>63</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C83" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E83" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F83" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G83" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3390,22 +3297,22 @@
         <v>64</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C84" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E84" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F84" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G84" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3413,22 +3320,22 @@
         <v>65</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C85" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D85" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E85" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F85" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G85" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3436,22 +3343,22 @@
         <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C86" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D86" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E86" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F86" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G86" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3459,22 +3366,22 @@
         <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D87" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E87" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F87" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G87" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3482,22 +3389,22 @@
         <v>68</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C88" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E88" t="s">
         <v>160</v>
       </c>
-      <c r="E88" t="s">
-        <v>166</v>
-      </c>
       <c r="F88" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="G88" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3505,22 +3412,22 @@
         <v>69</v>
       </c>
       <c r="B89" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C89" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D89" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E89" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F89" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G89" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3528,22 +3435,22 @@
         <v>70</v>
       </c>
       <c r="B90" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C90" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D90" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E90" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F90" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G90" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3551,22 +3458,22 @@
         <v>71</v>
       </c>
       <c r="B91" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C91" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D91" t="s">
+        <v>154</v>
+      </c>
+      <c r="E91" t="s">
         <v>160</v>
       </c>
-      <c r="E91" t="s">
-        <v>166</v>
-      </c>
       <c r="F91" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G91" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -3574,22 +3481,22 @@
         <v>72</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C92" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D92" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E92" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F92" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G92" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3597,22 +3504,22 @@
         <v>73</v>
       </c>
       <c r="B93" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C93" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D93" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E93" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F93" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G93" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3620,22 +3527,22 @@
         <v>73</v>
       </c>
       <c r="B94" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C94" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D94" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E94" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F94" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G94" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3643,22 +3550,22 @@
         <v>73</v>
       </c>
       <c r="B95" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C95" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D95" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E95" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F95" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G95" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3666,505 +3573,26 @@
         <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C96" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D96" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E96" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F96" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G96" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>61</v>
-      </c>
-      <c r="B97" t="s">
-        <v>139</v>
-      </c>
-      <c r="C97" t="s">
-        <v>158</v>
-      </c>
-      <c r="E97" t="s">
-        <v>166</v>
-      </c>
-      <c r="F97" t="s">
-        <v>261</v>
-      </c>
-      <c r="G97" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>75</v>
-      </c>
-      <c r="B98" t="s">
-        <v>153</v>
-      </c>
-      <c r="C98" t="s">
-        <v>158</v>
-      </c>
-      <c r="E98" t="s">
-        <v>163</v>
-      </c>
-      <c r="F98" t="s">
-        <v>262</v>
-      </c>
-      <c r="G98" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>76</v>
-      </c>
-      <c r="B99" t="s">
-        <v>154</v>
-      </c>
-      <c r="C99" t="s">
-        <v>158</v>
-      </c>
-      <c r="E99" t="s">
-        <v>163</v>
-      </c>
-      <c r="F99" t="s">
-        <v>262</v>
-      </c>
-      <c r="G99" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
-        <v>75</v>
-      </c>
-      <c r="B100" t="s">
-        <v>153</v>
-      </c>
-      <c r="C100" t="s">
-        <v>158</v>
-      </c>
-      <c r="E100" t="s">
-        <v>163</v>
-      </c>
-      <c r="F100" t="s">
-        <v>262</v>
-      </c>
-      <c r="G100" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
-        <v>75</v>
-      </c>
-      <c r="B101" t="s">
-        <v>153</v>
-      </c>
-      <c r="C101" t="s">
-        <v>158</v>
-      </c>
-      <c r="E101" t="s">
-        <v>163</v>
-      </c>
-      <c r="F101" t="s">
-        <v>262</v>
-      </c>
-      <c r="G101" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
-        <v>77</v>
-      </c>
-      <c r="B102" t="s">
-        <v>155</v>
-      </c>
-      <c r="C102" t="s">
-        <v>158</v>
-      </c>
-      <c r="E102" t="s">
-        <v>163</v>
-      </c>
-      <c r="F102" t="s">
-        <v>263</v>
-      </c>
-      <c r="G102" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
-        <v>77</v>
-      </c>
-      <c r="B103" t="s">
-        <v>155</v>
-      </c>
-      <c r="C103" t="s">
-        <v>158</v>
-      </c>
-      <c r="E103" t="s">
-        <v>163</v>
-      </c>
-      <c r="F103" t="s">
-        <v>264</v>
-      </c>
-      <c r="G103" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" t="s">
-        <v>75</v>
-      </c>
-      <c r="B104" t="s">
-        <v>153</v>
-      </c>
-      <c r="C104" t="s">
-        <v>158</v>
-      </c>
-      <c r="E104" t="s">
-        <v>163</v>
-      </c>
-      <c r="F104" t="s">
-        <v>262</v>
-      </c>
-      <c r="G104" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" t="s">
-        <v>75</v>
-      </c>
-      <c r="B105" t="s">
-        <v>153</v>
-      </c>
-      <c r="C105" t="s">
-        <v>158</v>
-      </c>
-      <c r="E105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F105" t="s">
-        <v>262</v>
-      </c>
-      <c r="G105" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" t="s">
-        <v>75</v>
-      </c>
-      <c r="B106" t="s">
-        <v>153</v>
-      </c>
-      <c r="C106" t="s">
-        <v>158</v>
-      </c>
-      <c r="E106" t="s">
-        <v>163</v>
-      </c>
-      <c r="F106" t="s">
-        <v>262</v>
-      </c>
-      <c r="G106" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" t="s">
-        <v>75</v>
-      </c>
-      <c r="B107" t="s">
-        <v>153</v>
-      </c>
-      <c r="C107" t="s">
-        <v>158</v>
-      </c>
-      <c r="E107" t="s">
-        <v>163</v>
-      </c>
-      <c r="F107" t="s">
-        <v>262</v>
-      </c>
-      <c r="G107" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
-        <v>75</v>
-      </c>
-      <c r="B108" t="s">
-        <v>153</v>
-      </c>
-      <c r="C108" t="s">
-        <v>158</v>
-      </c>
-      <c r="E108" t="s">
-        <v>163</v>
-      </c>
-      <c r="F108" t="s">
-        <v>262</v>
-      </c>
-      <c r="G108" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" t="s">
-        <v>75</v>
-      </c>
-      <c r="B109" t="s">
-        <v>153</v>
-      </c>
-      <c r="C109" t="s">
-        <v>158</v>
-      </c>
-      <c r="E109" t="s">
-        <v>163</v>
-      </c>
-      <c r="F109" t="s">
-        <v>262</v>
-      </c>
-      <c r="G109" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" t="s">
-        <v>75</v>
-      </c>
-      <c r="B110" t="s">
-        <v>153</v>
-      </c>
-      <c r="C110" t="s">
-        <v>158</v>
-      </c>
-      <c r="E110" t="s">
-        <v>163</v>
-      </c>
-      <c r="F110" t="s">
-        <v>262</v>
-      </c>
-      <c r="G110" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" t="s">
-        <v>75</v>
-      </c>
-      <c r="B111" t="s">
-        <v>153</v>
-      </c>
-      <c r="C111" t="s">
-        <v>158</v>
-      </c>
-      <c r="E111" t="s">
-        <v>163</v>
-      </c>
-      <c r="F111" t="s">
-        <v>262</v>
-      </c>
-      <c r="G111" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" t="s">
-        <v>77</v>
-      </c>
-      <c r="B112" t="s">
-        <v>155</v>
-      </c>
-      <c r="C112" t="s">
-        <v>158</v>
-      </c>
-      <c r="E112" t="s">
-        <v>163</v>
-      </c>
-      <c r="F112" t="s">
-        <v>264</v>
-      </c>
-      <c r="G112" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" t="s">
-        <v>75</v>
-      </c>
-      <c r="B113" t="s">
-        <v>153</v>
-      </c>
-      <c r="C113" t="s">
-        <v>158</v>
-      </c>
-      <c r="E113" t="s">
-        <v>163</v>
-      </c>
-      <c r="F113" t="s">
-        <v>262</v>
-      </c>
-      <c r="G113" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" t="s">
-        <v>77</v>
-      </c>
-      <c r="B114" t="s">
-        <v>155</v>
-      </c>
-      <c r="C114" t="s">
-        <v>158</v>
-      </c>
-      <c r="E114" t="s">
-        <v>163</v>
-      </c>
-      <c r="F114" t="s">
-        <v>263</v>
-      </c>
-      <c r="G114" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115" t="s">
-        <v>77</v>
-      </c>
-      <c r="B115" t="s">
-        <v>155</v>
-      </c>
-      <c r="C115" t="s">
-        <v>158</v>
-      </c>
-      <c r="E115" t="s">
-        <v>163</v>
-      </c>
-      <c r="F115" t="s">
-        <v>264</v>
-      </c>
-      <c r="G115" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="A116" t="s">
-        <v>77</v>
-      </c>
-      <c r="B116" t="s">
-        <v>155</v>
-      </c>
-      <c r="C116" t="s">
-        <v>158</v>
-      </c>
-      <c r="E116" t="s">
-        <v>163</v>
-      </c>
-      <c r="F116" t="s">
-        <v>263</v>
-      </c>
-      <c r="G116" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="A117" t="s">
-        <v>77</v>
-      </c>
-      <c r="B117" t="s">
-        <v>155</v>
-      </c>
-      <c r="C117" t="s">
-        <v>158</v>
-      </c>
-      <c r="E117" t="s">
-        <v>163</v>
-      </c>
-      <c r="F117" t="s">
-        <v>264</v>
-      </c>
-      <c r="G117" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118" t="s">
-        <v>75</v>
-      </c>
-      <c r="B118" t="s">
-        <v>153</v>
-      </c>
-      <c r="C118" t="s">
-        <v>158</v>
-      </c>
-      <c r="E118" t="s">
-        <v>163</v>
-      </c>
-      <c r="F118" t="s">
-        <v>262</v>
-      </c>
-      <c r="G118" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119" t="s">
-        <v>77</v>
-      </c>
-      <c r="B119" t="s">
-        <v>155</v>
-      </c>
-      <c r="C119" t="s">
-        <v>158</v>
-      </c>
-      <c r="E119" t="s">
-        <v>163</v>
-      </c>
-      <c r="F119" t="s">
-        <v>264</v>
-      </c>
-      <c r="G119" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" t="s">
-        <v>77</v>
-      </c>
-      <c r="B120" t="s">
-        <v>155</v>
-      </c>
-      <c r="C120" t="s">
-        <v>158</v>
-      </c>
-      <c r="E120" t="s">
-        <v>163</v>
-      </c>
-      <c r="F120" t="s">
-        <v>263</v>
-      </c>
-      <c r="G120" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>